<commit_message>
Laplace and Taubin smoothing
</commit_message>
<xml_diff>
--- a/book/theory/laplace_smoothing.xlsx
+++ b/book/theory/laplace_smoothing.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chovey/autotwin/automesh/book/theory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973BB58D-AAED-524D-A513-D9BD6C84BB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E259221F-A9C4-344E-8188-3A6F218E6274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26220" yWindow="2060" windowWidth="24920" windowHeight="17440" xr2:uid="{188DD368-EE4A-8442-9C16-133184D3B178}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{188DD368-EE4A-8442-9C16-133184D3B178}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>pbar</t>
-  </si>
-  <si>
     <t>pk</t>
   </si>
   <si>
-    <t>gk</t>
+    <t>lambda</t>
   </si>
   <si>
-    <t>lambda</t>
+    <t>qbar</t>
+  </si>
+  <si>
+    <t>Delta p k</t>
   </si>
 </sst>
 </file>
@@ -1463,14 +1463,14 @@
   <dimension ref="A4:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="E17" sqref="A7:E17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>0.3</v>
@@ -1478,13 +1478,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1498,12 +1498,12 @@
         <v>1.5</v>
       </c>
       <c r="D7">
-        <f>C7-B7</f>
-        <v>1</v>
+        <f>B7-C7</f>
+        <v>-1</v>
       </c>
       <c r="E7">
         <f>$F$4*D7</f>
-        <v>0.3</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1516,170 +1516,170 @@
         <v>0.5</v>
       </c>
       <c r="C8">
-        <f>C7-E7</f>
+        <f>C7+E7</f>
         <v>1.2</v>
       </c>
       <c r="D8">
-        <f>C8-B8</f>
-        <v>0.7</v>
+        <f t="shared" ref="D8:D17" si="0">B8-C8</f>
+        <v>-0.7</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E17" si="0">$F$4*D8</f>
-        <v>0.21</v>
+        <f t="shared" ref="E8:E17" si="1">$F$4*D8</f>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f t="shared" ref="A9:A17" si="1">1+A8</f>
+        <f t="shared" ref="A9:A17" si="2">1+A8</f>
         <v>2</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B17" si="2">B8</f>
+        <f t="shared" ref="B9:B17" si="3">B8</f>
         <v>0.5</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C17" si="3">C8-E8</f>
+        <f t="shared" ref="C9:C17" si="4">C8+E8</f>
         <v>0.99</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D17" si="4">C9-B9</f>
-        <v>0.49</v>
+        <f t="shared" si="0"/>
+        <v>-0.49</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0.14699999999999999</v>
+        <f t="shared" si="1"/>
+        <v>-0.14699999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="4"/>
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-0.34299999999999997</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="3"/>
-        <v>0.84299999999999997</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="4"/>
-        <v>0.34299999999999997</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0.10289999999999999</v>
+        <v>-0.10289999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="4"/>
+        <v>0.74009999999999998</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-0.24009999999999998</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="3"/>
-        <v>0.74009999999999998</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="4"/>
-        <v>0.24009999999999998</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>7.2029999999999997E-2</v>
+        <v>-7.2029999999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="4"/>
+        <v>0.66806999999999994</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-0.16806999999999994</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="3"/>
-        <v>0.66806999999999994</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="4"/>
-        <v>0.16806999999999994</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>5.042099999999998E-2</v>
+        <v>-5.042099999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="4"/>
+        <v>0.617649</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-0.117649</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="3"/>
-        <v>0.617649</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="4"/>
-        <v>0.117649</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>3.5294699999999998E-2</v>
+        <v>-3.5294699999999998E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="4"/>
+        <v>0.58235429999999999</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-8.2354299999999991E-2</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="3"/>
-        <v>0.58235429999999999</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="4"/>
-        <v>8.2354299999999991E-2</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>2.4706289999999995E-2</v>
+        <v>-2.4706289999999995E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="4"/>
+        <v>0.55764800999999997</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-5.7648009999999972E-2</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="3"/>
-        <v>0.55764800999999997</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="4"/>
-        <v>5.7648009999999972E-2</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1.7294402999999989E-2</v>
+        <v>-1.7294402999999989E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1688,42 +1688,42 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.54035360700000001</v>
       </c>
       <c r="D16">
-        <f t="shared" si="4"/>
-        <v>4.0353607000000014E-2</v>
+        <f t="shared" si="0"/>
+        <v>-4.0353607000000014E-2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>1.2106082100000004E-2</v>
+        <f t="shared" si="1"/>
+        <v>-1.2106082100000004E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="4"/>
+        <v>0.52824752490000004</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-2.8247524900000043E-2</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="3"/>
-        <v>0.52824752490000004</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="4"/>
-        <v>2.8247524900000043E-2</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>8.4742574700000118E-3</v>
+        <v>-8.4742574700000118E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>